<commit_message>
Editted 10th in 2nd task
</commit_message>
<xml_diff>
--- a/Problems 2.xlsx
+++ b/Problems 2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">Приведите пример супертипа сущности, не имеющего собственных экземпляров. </t>
   </si>
@@ -102,7 +102,13 @@
     <t>https://drive.google.com/file/d/1-UjP5o_cXXObYeU8K6GmdO_lM7LyvFR1/view?usp=sharing</t>
   </si>
   <si>
-    <t>intersect(self.категория_авто -&gt; название, self.водитель)  -&gt; size() &gt; 0</t>
+    <t>intersect (intersect (self.категория_авто , КатегорияАвтомобиля),</t>
+  </si>
+  <si>
+    <t>intersect (intersect (self.водитель, Водитель), intersect (self.водитель, КатегорияПравВодителя))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; size() &gt; 0</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -868,7 +874,7 @@
       <c r="I47" s="5"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="49" spans="2:8">
+    <row r="49" spans="2:12">
       <c r="B49" s="8" t="s">
         <v>24</v>
       </c>
@@ -877,18 +883,56 @@
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="13" t="s">
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="10"/>
+    </row>
+    <row r="50" spans="2:12">
+      <c r="B50" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="14"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="12"/>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="11"/>
+      <c r="C51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="12"/>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="B52" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>